<commit_message>
starting adding resutls with RF
</commit_message>
<xml_diff>
--- a/results/Comparison.xlsx
+++ b/results/Comparison.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
-  <si>
-    <t xml:space="preserve">ALL THESE TABLES ARE THE RESULT OF APPLYING DECISION TREE AS CLASSIFIER</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">USING DECISION TREE AS CLASSIFIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USING RANDOM FOREST AS CLASSIFIER</t>
   </si>
   <si>
     <t xml:space="preserve">TEST</t>
@@ -87,11 +90,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -109,25 +113,14 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -181,16 +174,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -198,15 +191,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -227,54 +216,78 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C2:G31"/>
+  <dimension ref="C2:O31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>335.522344375</v>
@@ -285,13 +298,19 @@
       <c r="F7" s="0" t="n">
         <v>294.197835</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="1" t="n">
         <v>293.04720425</v>
       </c>
+      <c r="K7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="O7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>507.864773125</v>
@@ -302,13 +321,19 @@
       <c r="F8" s="0" t="n">
         <v>504.247715</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="1" t="n">
         <v>477.024043499999</v>
       </c>
+      <c r="K8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="O8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>5.04009125</v>
@@ -322,10 +347,15 @@
       <c r="G9" s="0" t="n">
         <v>0.600813749999999</v>
       </c>
+      <c r="K9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>5.04321</v>
@@ -336,13 +366,19 @@
       <c r="F10" s="0" t="n">
         <v>0.6146425</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="1" t="n">
         <v>0.6127</v>
       </c>
+      <c r="K10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="O10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>79.86608875</v>
@@ -351,15 +387,21 @@
         <v>68.365613125</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>68.1876514999999</v>
+      </c>
+      <c r="K11" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="2" t="n">
-        <v>68.1876514999999</v>
-      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+      <c r="O11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>93.221359375</v>
@@ -370,18 +412,24 @@
       <c r="F12" s="0" t="n">
         <v>84.9192025</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="1" t="n">
         <v>84.200227125</v>
       </c>
+      <c r="K12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="O12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>0.901333571428571</v>
       </c>
-      <c r="E13" s="6" t="n">
+      <c r="E13" s="5" t="n">
         <v>0.861159285714286</v>
       </c>
       <c r="F13" s="0" t="n">
@@ -390,10 +438,15 @@
       <c r="G13" s="0" t="n">
         <v>0.867441857142857</v>
       </c>
+      <c r="K13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>2987.28098333333</v>
@@ -404,10 +457,15 @@
       <c r="F14" s="0" t="n">
         <v>2992.45627333333</v>
       </c>
+      <c r="K14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="2" t="s">
-        <v>17</v>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">AVERAGE(D7:D13)</f>
@@ -425,35 +483,75 @@
         <f aca="false">AVERAGE(G7:G13)</f>
         <v>132.077154568877</v>
       </c>
+      <c r="K15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="0" t="e">
+        <f aca="false">AVERAGE(L7:L13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="0" t="e">
+        <f aca="false">AVERAGE(M7:M13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="0" t="e">
+        <f aca="false">AVERAGE(N7:N13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="0" t="e">
+        <f aca="false">AVERAGE(O7:O13)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>18</v>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D23" s="3" t="n">
         <v>1449696.48115875</v>
@@ -464,18 +562,24 @@
       <c r="F23" s="0" t="n">
         <v>1022735.09378</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="G23" s="1" t="n">
         <v>969418.822309125</v>
       </c>
+      <c r="K23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="O23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>2114498.78511125</v>
       </c>
-      <c r="E24" s="6" t="n">
+      <c r="E24" s="5" t="n">
         <v>1904021.83070375</v>
       </c>
       <c r="F24" s="0" t="n">
@@ -484,10 +588,15 @@
       <c r="G24" s="0" t="n">
         <v>1921188.99825175</v>
       </c>
+      <c r="K24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D25" s="4" t="n">
         <v>210.33799125</v>
@@ -495,16 +604,22 @@
       <c r="E25" s="4" t="n">
         <v>4.8013175</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" s="1" t="n">
         <v>3.251645</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>3.576215</v>
       </c>
+      <c r="K25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D26" s="4" t="n">
         <v>210.275505</v>
@@ -515,13 +630,19 @@
       <c r="F26" s="0" t="n">
         <v>5.74483625</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G26" s="1" t="n">
         <v>3.60863</v>
       </c>
+      <c r="K26" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="O26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>15357.2590825</v>
@@ -530,15 +651,21 @@
         <v>13034.343416875</v>
       </c>
       <c r="F27" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>12721.214303125</v>
+      </c>
+      <c r="K27" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="2" t="n">
-        <v>12721.214303125</v>
-      </c>
+      <c r="L27" s="3"/>
+      <c r="M27" s="4"/>
+      <c r="O27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D28" s="4" t="n">
         <v>20866.32091625</v>
@@ -549,13 +676,19 @@
       <c r="F28" s="0" t="n">
         <v>19113.97089</v>
       </c>
-      <c r="G28" s="2" t="n">
+      <c r="G28" s="1" t="n">
         <v>18963.374284375</v>
       </c>
+      <c r="K28" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="O28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D29" s="3" t="n">
         <v>1.54834428571429</v>
@@ -563,16 +696,22 @@
       <c r="E29" s="3" t="n">
         <v>1.55736285714286</v>
       </c>
-      <c r="F29" s="2" t="n">
+      <c r="F29" s="1" t="n">
         <v>1.52703</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>1.52870171428571</v>
       </c>
+      <c r="K29" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D30" s="3" t="n">
         <f aca="false">3.53917960778694*10^7</f>
@@ -586,10 +725,15 @@
         <f aca="false">3.61565476474173*10^7</f>
         <v>36156547.6474173</v>
       </c>
+      <c r="K30" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="2" t="s">
-        <v>17</v>
+      <c r="C31" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D31" s="0" t="n">
         <f aca="false">AVERAGE(D23:D29)</f>
@@ -606,6 +750,25 @@
       <c r="G31" s="0" t="n">
         <f aca="false">AVERAGE(G23:G29)</f>
         <v>417471.588956441</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" s="0" t="e">
+        <f aca="false">AVERAGE(L23:L29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M31" s="0" t="e">
+        <f aca="false">AVERAGE(M23:M29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N31" s="0" t="e">
+        <f aca="false">AVERAGE(N23:N29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O31" s="0" t="e">
+        <f aca="false">AVERAGE(O23:O29)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results on Olfacion data
</commit_message>
<xml_diff>
--- a/results/Comparison.xlsx
+++ b/results/Comparison.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="22">
   <si>
     <t xml:space="preserve">USING DECISION TREE AS CLASSIFIER</t>
   </si>
   <si>
     <t xml:space="preserve">USING RANDOM FOREST AS CLASSIFIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uses 50 trees</t>
   </si>
   <si>
     <t xml:space="preserve">TEST</t>
@@ -93,7 +96,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -118,6 +121,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -177,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,7 +197,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,18 +234,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C2:O31"/>
+  <dimension ref="C2:P31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P29" activeCellId="0" sqref="P29"/>
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -240,61 +258,64 @@
       <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="P2" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="O6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="n">
         <v>335.522344375</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>335.536215625</v>
       </c>
       <c r="F7" s="0" t="n">
@@ -304,12 +325,12 @@
         <v>293.04720425</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L7" s="4" t="n">
         <v>240.693775</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="M7" s="4" t="n">
         <v>227.7623975</v>
       </c>
       <c r="N7" s="0" t="n">
@@ -319,12 +340,12 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="n">
         <v>507.864773125</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="4" t="n">
         <v>480.957105625</v>
       </c>
       <c r="F8" s="0" t="n">
@@ -334,12 +355,12 @@
         <v>477.024043499999</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="L8" s="4" t="n">
         <v>395.100456875</v>
       </c>
-      <c r="M8" s="3" t="n">
+      <c r="M8" s="4" t="n">
         <v>379.34393125</v>
       </c>
       <c r="N8" s="0" t="n">
@@ -349,12 +370,12 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="n">
         <v>5.04009125</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="6" t="n">
         <v>0.60032875</v>
       </c>
       <c r="F9" s="0" t="n">
@@ -364,12 +385,12 @@
         <v>0.600813749999999</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="L9" s="4" t="n">
         <v>0.42858</v>
       </c>
-      <c r="M9" s="3" t="n">
+      <c r="M9" s="4" t="n">
         <v>0.412795</v>
       </c>
       <c r="N9" s="0" t="n">
@@ -378,12 +399,12 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5" t="n">
         <v>5.04321</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="5" t="n">
         <v>0.61703625</v>
       </c>
       <c r="F10" s="0" t="n">
@@ -393,12 +414,12 @@
         <v>0.6127</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="L10" s="4" t="n">
         <v>0.87113</v>
       </c>
-      <c r="M10" s="3" t="n">
+      <c r="M10" s="4" t="n">
         <v>0.7214025</v>
       </c>
       <c r="N10" s="0" t="n">
@@ -408,42 +429,42 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="D11" s="4" t="n">
         <v>79.86608875</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="5" t="n">
         <v>68.365613125</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1" t="n">
         <v>68.1876514999999</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="L11" s="4" t="n">
         <v>53.58701125</v>
       </c>
-      <c r="M11" s="3" t="n">
+      <c r="M11" s="4" t="n">
         <v>49.55937625</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>93.221359375</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E12" s="5" t="n">
         <v>85.27151</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -453,27 +474,27 @@
         <v>84.200227125</v>
       </c>
       <c r="K12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="4" t="n">
+        <v>66.070739375</v>
+      </c>
+      <c r="M12" s="4" t="n">
+        <v>64.81183875</v>
+      </c>
+      <c r="N12" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="L12" s="3" t="n">
-        <v>66.070739375</v>
-      </c>
-      <c r="M12" s="3" t="n">
-        <v>64.81183875</v>
-      </c>
-      <c r="N12" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="O12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="n">
         <v>0.901333571428571</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="6" t="n">
         <v>0.861159285714286</v>
       </c>
       <c r="F13" s="0" t="n">
@@ -483,12 +504,12 @@
         <v>0.867441857142857</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="L13" s="5" t="n">
         <v>0.832445714285714</v>
       </c>
-      <c r="M13" s="4" t="n">
+      <c r="M13" s="5" t="n">
         <v>0.825584285714286</v>
       </c>
       <c r="N13" s="0" t="n">
@@ -497,24 +518,24 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="D14" s="4" t="n">
         <v>2987.28098333333</v>
       </c>
-      <c r="E14" s="3" t="n">
+      <c r="E14" s="4" t="n">
         <v>3270.1264875</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>2992.45627333333</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L14" s="0" t="n">
         <v>2959.88022583333</v>
       </c>
-      <c r="M14" s="3" t="n">
+      <c r="M14" s="4" t="n">
         <v>2938.12863416667</v>
       </c>
       <c r="N14" s="0" t="n">
@@ -523,7 +544,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">AVERAGE(D7:D14)</f>
@@ -542,7 +563,7 @@
         <v>132.077154568877</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L15" s="0" t="n">
         <f aca="false">AVERAGE(L7:L14)</f>
@@ -562,59 +583,59 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>20</v>
+      <c r="C20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K22" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="O22" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D23" s="4" t="n">
         <v>1449696.48115875</v>
       </c>
-      <c r="E23" s="3" t="n">
+      <c r="E23" s="4" t="n">
         <v>1508252.23498125</v>
       </c>
       <c r="F23" s="0" t="n">
@@ -624,12 +645,12 @@
         <v>969418.822309125</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="L23" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L23" s="4" t="n">
         <v>532364.60696375</v>
       </c>
-      <c r="M23" s="4" t="n">
+      <c r="M23" s="5" t="n">
         <v>531129.18718375</v>
       </c>
       <c r="N23" s="0" t="n">
@@ -639,12 +660,12 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="D24" s="4" t="n">
         <v>2114498.78511125</v>
       </c>
-      <c r="E24" s="5" t="n">
+      <c r="E24" s="6" t="n">
         <v>1904021.83070375</v>
       </c>
       <c r="F24" s="0" t="n">
@@ -654,12 +675,12 @@
         <v>1921188.99825175</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="L24" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="L24" s="4" t="n">
         <v>974421.037385</v>
       </c>
-      <c r="M24" s="4" t="n">
+      <c r="M24" s="5" t="n">
         <v>915283.118903125</v>
       </c>
       <c r="N24" s="0" t="n">
@@ -668,12 +689,12 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D25" s="5" t="n">
         <v>210.33799125</v>
       </c>
-      <c r="E25" s="4" t="n">
+      <c r="E25" s="5" t="n">
         <v>4.8013175</v>
       </c>
       <c r="F25" s="1" t="n">
@@ -683,12 +704,12 @@
         <v>3.576215</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="L25" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="L25" s="4" t="n">
         <v>2.30629</v>
       </c>
-      <c r="M25" s="4" t="n">
+      <c r="M25" s="5" t="n">
         <v>1.5901125</v>
       </c>
       <c r="N25" s="0" t="n">
@@ -697,12 +718,12 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="D26" s="5" t="n">
         <v>210.275505</v>
       </c>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="5" t="n">
         <v>4.1802525</v>
       </c>
       <c r="F26" s="0" t="n">
@@ -712,12 +733,12 @@
         <v>3.60863</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="L26" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="L26" s="4" t="n">
         <v>7.3471375</v>
       </c>
-      <c r="M26" s="4" t="n">
+      <c r="M26" s="5" t="n">
         <v>4.73616625</v>
       </c>
       <c r="N26" s="0" t="n">
@@ -727,42 +748,42 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="D27" s="4" t="n">
         <v>15357.2590825</v>
       </c>
-      <c r="E27" s="4" t="n">
+      <c r="E27" s="5" t="n">
         <v>13034.343416875</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G27" s="1" t="n">
         <v>12721.214303125</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="L27" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="L27" s="4" t="n">
         <v>7323.444506875</v>
       </c>
-      <c r="M27" s="4" t="n">
+      <c r="M27" s="5" t="n">
         <v>6601.73254125</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="D28" s="5" t="n">
         <v>20866.32091625</v>
       </c>
-      <c r="E28" s="4" t="n">
+      <c r="E28" s="5" t="n">
         <v>20135.445213125</v>
       </c>
       <c r="F28" s="0" t="n">
@@ -772,27 +793,27 @@
         <v>18963.374284375</v>
       </c>
       <c r="K28" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="4" t="n">
+        <v>9864.792405</v>
+      </c>
+      <c r="M28" s="5" t="n">
+        <v>9742.48709375</v>
+      </c>
+      <c r="N28" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="L28" s="3" t="n">
-        <v>9864.792405</v>
-      </c>
-      <c r="M28" s="4" t="n">
-        <v>9742.48709375</v>
-      </c>
-      <c r="N28" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="O28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="D29" s="4" t="n">
         <v>1.54834428571429</v>
       </c>
-      <c r="E29" s="3" t="n">
+      <c r="E29" s="4" t="n">
         <v>1.55736285714286</v>
       </c>
       <c r="F29" s="1" t="n">
@@ -802,12 +823,12 @@
         <v>1.52870171428571</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="L29" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="L29" s="5" t="n">
         <v>1.35214428571429</v>
       </c>
-      <c r="M29" s="4" t="n">
+      <c r="M29" s="5" t="n">
         <v>1.353015</v>
       </c>
       <c r="N29" s="0" t="n">
@@ -816,13 +837,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="D30" s="4" t="n">
         <f aca="false">3.53917960778694*10^7</f>
         <v>35391796.0778694</v>
       </c>
-      <c r="E30" s="3" t="n">
+      <c r="E30" s="4" t="n">
         <f aca="false">4.28651928502041*10^7</f>
         <v>42865192.8502041</v>
       </c>
@@ -831,13 +852,13 @@
         <v>36156547.6474173</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L30" s="0" t="n">
         <f aca="false">3.95277925178316*10^7</f>
         <v>39527792.5178316</v>
       </c>
-      <c r="M30" s="3" t="n">
+      <c r="M30" s="4" t="n">
         <f aca="false">3.15486468098213*10^7</f>
         <v>31548646.8098213</v>
       </c>
@@ -848,7 +869,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D31" s="0" t="n">
         <f aca="false">AVERAGE(D23:D30)</f>
@@ -867,7 +888,7 @@
         <v>417471.588956441</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L31" s="0" t="n">
         <f aca="false">AVERAGE(L23:L30)</f>

</xml_diff>

<commit_message>
new results plus statistics
</commit_message>
<xml_diff>
--- a/results/Comparison.xlsx
+++ b/results/Comparison.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
   <si>
     <t>USING DECISION TREE AS CLASSIFIER</t>
   </si>
@@ -96,14 +96,24 @@
   </si>
   <si>
     <t>MSE</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>GA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -160,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -169,6 +179,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,15 +462,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:P31"/>
+  <dimension ref="C2:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5:U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="12" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:16" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:27" ht="18" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
@@ -479,7 +498,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="3:27" x14ac:dyDescent="0.15">
+      <c r="S5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="Y5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+    </row>
+    <row r="6" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -510,8 +541,26 @@
       <c r="O6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.15">
+      <c r="S6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
         <v>10</v>
       </c>
@@ -542,8 +591,26 @@
       <c r="O7">
         <v>229.98624375</v>
       </c>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.15">
+      <c r="S7" s="8">
+        <v>240.69377499999999</v>
+      </c>
+      <c r="T7" s="9">
+        <v>227.76239749999999</v>
+      </c>
+      <c r="U7" s="8">
+        <v>229.98624375</v>
+      </c>
+      <c r="Y7" s="8">
+        <v>335.52234437499999</v>
+      </c>
+      <c r="Z7" s="8">
+        <v>335.53621562500001</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>293.04720424999999</v>
+      </c>
+    </row>
+    <row r="8" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -574,8 +641,26 @@
       <c r="O8">
         <v>385.13324875000001</v>
       </c>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.15">
+      <c r="S8" s="8">
+        <v>395.10045687500002</v>
+      </c>
+      <c r="T8" s="9">
+        <v>379.34393125000003</v>
+      </c>
+      <c r="U8" s="8">
+        <v>385.13324875000001</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>507.864773125</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>480.957105625</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>477.02404349999898</v>
+      </c>
+    </row>
+    <row r="9" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C9" t="s">
         <v>12</v>
       </c>
@@ -606,8 +691,26 @@
       <c r="O9">
         <v>0.417603749999999</v>
       </c>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.15">
+      <c r="S9" s="8">
+        <v>0.42858000000000002</v>
+      </c>
+      <c r="T9" s="9">
+        <v>0.41279500000000002</v>
+      </c>
+      <c r="U9" s="8">
+        <v>0.417603749999999</v>
+      </c>
+      <c r="Y9" s="10">
+        <v>5.0400912499999997</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>0.60032874999999997</v>
+      </c>
+      <c r="AA9" s="8">
+        <v>0.60081374999999904</v>
+      </c>
+    </row>
+    <row r="10" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -638,8 +741,26 @@
       <c r="O10">
         <v>0.77481250000000002</v>
       </c>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.15">
+      <c r="S10" s="8">
+        <v>0.87112999999999996</v>
+      </c>
+      <c r="T10" s="9">
+        <v>0.72140249999999995</v>
+      </c>
+      <c r="U10" s="8">
+        <v>0.77481250000000002</v>
+      </c>
+      <c r="Y10" s="10">
+        <v>5.0432100000000002</v>
+      </c>
+      <c r="Z10" s="10">
+        <v>0.61703624999999995</v>
+      </c>
+      <c r="AA10" s="9">
+        <v>0.61270000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C11" t="s">
         <v>14</v>
       </c>
@@ -670,8 +791,26 @@
       <c r="O11">
         <v>49.738267499999999</v>
       </c>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.15">
+      <c r="S11" s="8">
+        <v>53.587011250000003</v>
+      </c>
+      <c r="T11" s="9">
+        <v>49.55937625</v>
+      </c>
+      <c r="U11" s="8">
+        <v>49.738267499999999</v>
+      </c>
+      <c r="Y11" s="8">
+        <v>79.866088750000003</v>
+      </c>
+      <c r="Z11" s="10">
+        <v>68.365613124999996</v>
+      </c>
+      <c r="AA11" s="9">
+        <v>68.187651499999902</v>
+      </c>
+    </row>
+    <row r="12" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C12" t="s">
         <v>17</v>
       </c>
@@ -702,8 +841,26 @@
       <c r="O12">
         <v>64.859575625000005</v>
       </c>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.15">
+      <c r="S12" s="8">
+        <v>66.070739375000002</v>
+      </c>
+      <c r="T12" s="9">
+        <v>64.811838750000007</v>
+      </c>
+      <c r="U12" s="8">
+        <v>64.859575625000005</v>
+      </c>
+      <c r="Y12" s="10">
+        <v>93.221359375000006</v>
+      </c>
+      <c r="Z12" s="10">
+        <v>85.271510000000006</v>
+      </c>
+      <c r="AA12" s="9">
+        <v>84.200227124999998</v>
+      </c>
+    </row>
+    <row r="13" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C13" t="s">
         <v>18</v>
       </c>
@@ -734,8 +891,26 @@
       <c r="O13" s="1">
         <v>0.82457499999999995</v>
       </c>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.15">
+      <c r="S13" s="10">
+        <v>0.83244571428571401</v>
+      </c>
+      <c r="T13" s="10">
+        <v>0.82558428571428599</v>
+      </c>
+      <c r="U13" s="9">
+        <v>0.82457499999999995</v>
+      </c>
+      <c r="Y13" s="8">
+        <v>0.90133357142857096</v>
+      </c>
+      <c r="Z13" s="9">
+        <v>0.86115928571428602</v>
+      </c>
+      <c r="AA13" s="8">
+        <v>0.86744185714285704</v>
+      </c>
+    </row>
+    <row r="14" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C14" t="s">
         <v>19</v>
       </c>
@@ -748,7 +923,7 @@
       <c r="F14">
         <v>2992.45627333333</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>2945.4223541666602</v>
       </c>
       <c r="K14" t="s">
@@ -757,7 +932,7 @@
       <c r="L14">
         <v>2959.8802258333299</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="6">
         <v>2938.1286341666701</v>
       </c>
       <c r="N14">
@@ -766,8 +941,26 @@
       <c r="O14">
         <v>2945.4223541666602</v>
       </c>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.15">
+      <c r="S14" s="8">
+        <v>2959.8802258333299</v>
+      </c>
+      <c r="T14" s="9">
+        <v>2938.1286341666701</v>
+      </c>
+      <c r="U14" s="8">
+        <v>2945.4223541666602</v>
+      </c>
+      <c r="Y14" s="8">
+        <v>2987.2809833333299</v>
+      </c>
+      <c r="Z14" s="8">
+        <v>3270.1264875000002</v>
+      </c>
+      <c r="AA14" s="9">
+        <v>2945.4223541666602</v>
+      </c>
+    </row>
+    <row r="15" spans="3:27" x14ac:dyDescent="0.15">
       <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1156,6 +1349,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="Y5:AA5"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>

</xml_diff>